<commit_message>
fix hearing value sets
</commit_message>
<xml_diff>
--- a/output/ValueSet-SPLASCHHearingObservationValueVS.xlsx
+++ b/output/ValueSet-SPLASCHHearingObservationValueVS.xlsx
@@ -7,17 +7,19 @@
   </bookViews>
   <sheets>
     <sheet name="Metadata" r:id="rId3" sheetId="1"/>
-    <sheet name="Include ValueSets" r:id="rId4" sheetId="2"/>
-    <sheet name="Include ValueSets 2" r:id="rId5" sheetId="3"/>
-    <sheet name="Include ValueSets 3" r:id="rId6" sheetId="4"/>
-    <sheet name="Include ValueSets 4" r:id="rId7" sheetId="5"/>
-    <sheet name="Include ValueSets 5" r:id="rId8" sheetId="6"/>
+    <sheet name="Include from Hearing Loss - T" r:id="rId4" sheetId="2"/>
+    <sheet name="Include from Hearing Loss - D" r:id="rId5" sheetId="3"/>
+    <sheet name="Include ValueSets" r:id="rId6" sheetId="4"/>
+    <sheet name="Include ValueSets 2" r:id="rId7" sheetId="5"/>
+    <sheet name="Include ValueSets 3" r:id="rId8" sheetId="6"/>
+    <sheet name="Include ValueSets 4" r:id="rId9" sheetId="7"/>
+    <sheet name="Include ValueSets 5" r:id="rId10" sheetId="8"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="40">
   <si>
     <t>Property</t>
   </si>
@@ -61,7 +63,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-05-04T09:54:10-04:00</t>
+    <t>2022-05-04T12:01:11-04:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -101,6 +103,24 @@
   </si>
   <si>
     <t>BooleanType[null]</t>
+  </si>
+  <si>
+    <t>Codes</t>
+  </si>
+  <si>
+    <t>All codes</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>System URI</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/pacio-splasch/CodeSystem/HearingLossTypeCS</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/pacio-splasch/CodeSystem/HearingLossDegreeCS</t>
   </si>
   <si>
     <t>ValueSet URL</t>
@@ -393,7 +413,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -413,6 +433,22 @@
         <v>29</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="s" s="2">
+        <v>30</v>
+      </c>
+      <c r="B3" t="s" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="2">
+        <v>31</v>
+      </c>
+      <c r="B4" t="s" s="2">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -420,7 +456,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -437,7 +473,23 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="2">
         <v>30</v>
+      </c>
+      <c r="B3" t="s" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="2">
+        <v>31</v>
+      </c>
+      <c r="B4" t="s" s="2">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -459,12 +511,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="1">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s" s="2">
-        <v>31</v>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="2">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -486,12 +538,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="1">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s" s="2">
-        <v>32</v>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="2">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -513,12 +565,66 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="1">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s" s="2">
-        <v>33</v>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="2">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" width="30.703125" customWidth="true"/>
+    <col min="2" max="2" width="50.703125" customWidth="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="1">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="2">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" width="30.703125" customWidth="true"/>
+    <col min="2" max="2" width="50.703125" customWidth="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="1">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="2">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>